<commit_message>
Final statistics and bugfixes
</commit_message>
<xml_diff>
--- a/Ejecuciones.xlsx
+++ b/Ejecuciones.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27660" yWindow="8820" windowWidth="22220" windowHeight="16880" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="24000" yWindow="3580" windowWidth="22220" windowHeight="16880" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="10">
   <si>
     <t>Mapa</t>
   </si>
@@ -59,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +88,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -106,7 +112,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -128,8 +134,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -138,8 +150,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="27">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -150,6 +168,9 @@
     <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -160,9 +181,113 @@
     <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -712,44 +837,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="34" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
+    <row r="1" spans="1:7" ht="34" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="5">
         <v>3</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="5">
         <v>9</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="5">
         <v>12</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="5">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" ht="34" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -765,21 +886,31 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="34" customHeight="1">
-      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="34" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="34" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="34" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -795,20 +926,185 @@
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="34" customHeight="1">
-      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="34" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="str">
+        <f>(IF(COUNTIF(B2:B5,"=IA")=4,"IA","IA/Base"))</f>
+        <v>IA</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f t="shared" ref="C6:F6" si="0">(IF(COUNTIF(C2:C5,"=IA")=4,"IA","IA/Base"))</f>
+        <v>IA</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>IA</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>IA</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>IA/Base</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="34" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="34" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="34" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="34" customHeight="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2" t="str">
+        <f>(IF(COUNTIF(B8:B11,"=IA")=4,"IA","IA/Base"))</f>
+        <v>IA</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f t="shared" ref="C12" si="1">(IF(COUNTIF(C8:C11,"=IA")=4,"IA","IA/Base"))</f>
+        <v>IA</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f t="shared" ref="D12" si="2">(IF(COUNTIF(D8:D11,"=IA")=4,"IA","IA/Base"))</f>
+        <v>IA</v>
+      </c>
+      <c r="E12" s="2" t="str">
+        <f t="shared" ref="E12" si="3">(IF(COUNTIF(E8:E11,"=IA")=4,"IA","IA/Base"))</f>
+        <v>IA</v>
+      </c>
+      <c r="F12" s="2" t="str">
+        <f t="shared" ref="F12" si="4">(IF(COUNTIF(F8:F11,"=IA")=4,"IA","IA/Base"))</f>
+        <v>IA/Base</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:F12 G5">
+    <cfRule type="endsWith" dxfId="7" priority="1" operator="endsWith" text="Base">
+      <formula>RIGHT(B1,LEN("Base"))="Base"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="8" priority="2" operator="endsWith" text="IA">
+      <formula>RIGHT(B1,LEN("IA"))="IA"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -823,7 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>

</xml_diff>